<commit_message>
Added cover headline verbiages
</commit_message>
<xml_diff>
--- a/Career Spread.xlsx
+++ b/Career Spread.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arun\source\repos\personal-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A062C81F-F4A1-4DE4-B49C-C18EEB889DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8788BE8-AE9C-4198-B579-F9F1820D01C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{0B431C5F-1814-4948-8F9E-210218A3D24B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Months</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>Year 2023</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Year 2024</t>
+  </si>
+  <si>
+    <t>Year 2025</t>
   </si>
 </sst>
 </file>
@@ -147,12 +159,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,15 +480,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE88C20-C6ED-4227-A0F5-404ACB46CF1B}">
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B6"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -539,8 +552,14 @@
       <c r="U1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="V1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>37803</v>
       </c>
@@ -598,8 +617,11 @@
       </c>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="V2" s="1">
+        <v>45108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>37834</v>
       </c>
@@ -656,11 +678,12 @@
         <v>44409</v>
       </c>
       <c r="T3" s="4"/>
-      <c r="U3" s="1">
+      <c r="U3" s="4"/>
+      <c r="V3" s="1">
         <v>45139</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>37865</v>
       </c>
@@ -717,11 +740,12 @@
         <v>44440</v>
       </c>
       <c r="T4" s="4"/>
-      <c r="U4" s="1">
+      <c r="U4" s="4"/>
+      <c r="V4" s="1">
         <v>45170</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>37895</v>
       </c>
@@ -781,8 +805,11 @@
       <c r="U5" s="1">
         <v>45200</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="V5" s="1">
+        <v>45200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>37926</v>
       </c>
@@ -842,8 +869,11 @@
       <c r="U6" s="1">
         <v>45231</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="V6" s="1">
+        <v>45231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>37956</v>
       </c>
@@ -905,8 +935,11 @@
       <c r="U7" s="1">
         <v>45261</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="V7" s="1">
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>37987</v>
       </c>
@@ -968,8 +1001,11 @@
       <c r="U8" s="1">
         <v>45292</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="V8" s="1">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>38018</v>
       </c>
@@ -1031,8 +1067,11 @@
       <c r="U9" s="1">
         <v>45323</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="V9" s="1">
+        <v>45323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>38047</v>
       </c>
@@ -1094,8 +1133,11 @@
       <c r="U10" s="1">
         <v>45352</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="V10" s="1">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>38078</v>
       </c>
@@ -1155,8 +1197,11 @@
       <c r="U11" s="1">
         <v>45383</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="V11" s="1">
+        <v>45383</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>38108</v>
       </c>
@@ -1216,8 +1261,11 @@
       <c r="U12" s="1">
         <v>45413</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="V12" s="1">
+        <v>45413</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>38139</v>
       </c>
@@ -1277,8 +1325,11 @@
       <c r="U13" s="1">
         <v>45444</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="V13" s="1">
+        <v>45444</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <f>COUNTA(A2:A13)</f>
         <v>12</v>
@@ -1361,14 +1412,14 @@
       </c>
       <c r="U14">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="R16" t="s">
         <v>0</v>
       </c>
@@ -1381,12 +1432,80 @@
         <v>18.333333333333332</v>
       </c>
     </row>
-    <row r="18" spans="18:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="4:19" x14ac:dyDescent="0.55000000000000004">
       <c r="R18" t="s">
         <v>1</v>
       </c>
       <c r="S18">
         <v>18.3</v>
+      </c>
+    </row>
+    <row r="21" spans="4:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="4:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="D22">
+        <v>3309250</v>
+      </c>
+      <c r="E22">
+        <f>20%*D22</f>
+        <v>661850</v>
+      </c>
+      <c r="G22">
+        <f>D22+E22</f>
+        <v>3971100</v>
+      </c>
+      <c r="H22">
+        <f>G22*20%</f>
+        <v>794220</v>
+      </c>
+    </row>
+    <row r="23" spans="4:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="D23" s="5">
+        <v>222513</v>
+      </c>
+      <c r="E23">
+        <f>D22+E22</f>
+        <v>3971100</v>
+      </c>
+      <c r="F23" s="5">
+        <f>E23+D23</f>
+        <v>4193613</v>
+      </c>
+      <c r="H23">
+        <f>G22+H22</f>
+        <v>4765320</v>
+      </c>
+    </row>
+    <row r="24" spans="4:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="D24">
+        <f>SUM(D22:D23)</f>
+        <v>3531763</v>
+      </c>
+      <c r="H24">
+        <f>D24*20%</f>
+        <v>706352.60000000009</v>
+      </c>
+    </row>
+    <row r="25" spans="4:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="H25">
+        <f>D24+H24</f>
+        <v>4238115.5999999996</v>
+      </c>
+      <c r="I25">
+        <f>H25*20%</f>
+        <v>847623.12</v>
+      </c>
+    </row>
+    <row r="26" spans="4:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="I26">
+        <f>H25+I25</f>
+        <v>5085738.72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>